<commit_message>
fixed test error 3
</commit_message>
<xml_diff>
--- a/tests/data/20250305_experiment_file.xlsx
+++ b/tests/data/20250305_experiment_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop-PC\PycharmProjects\nomad-hysprint\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB17D7A1-13D6-433B-8F34-5988C92EB259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E75FB83-0B3C-49F2-86A2-0C062F70EC72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1025,7 +1025,7 @@
   <dimension ref="A1:GY18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:H18"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>